<commit_message>
Updated REV4 to include fuse & input polarity protection
</commit_message>
<xml_diff>
--- a/Arduino_Shield_REV4_BOM.xlsx
+++ b/Arduino_Shield_REV4_BOM.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3480" yWindow="480" windowWidth="24380" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="3480" yWindow="460" windowWidth="24380" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Arduino_Shield_6_5_19_REV4_BOM" localSheetId="0">Sheet2!$A$1:$I$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$A$1:$A$49</definedName>
+    <definedName name="Arduino_Shield_6_5_19_REV4_BOM" localSheetId="0">Sheet2!$A$1:$I$42</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -52,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="180">
   <si>
     <t>Part</t>
   </si>
@@ -285,21 +286,6 @@
     <t>TX</t>
   </si>
   <si>
-    <t>U$2</t>
-  </si>
-  <si>
-    <t>SKM15C-12_DCDC</t>
-  </si>
-  <si>
-    <t>Isolated DC/DC Converters 15W 36-75Vin 12Vout 125-1250mA 1x1 size</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/MEAN-WELL/SKM15C-12?qs=%2Fha2pyFaduhh55LLYaK%2FKJ2VcEvgwt5xUEx7a8eNZIE%3D</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> SKM15C-12</t>
-  </si>
-  <si>
     <t>RESONATOR</t>
   </si>
   <si>
@@ -514,6 +500,99 @@
   </si>
   <si>
     <t>C11</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>ZENER</t>
+  </si>
+  <si>
+    <t>ZENER_DIODE</t>
+  </si>
+  <si>
+    <t>Zener Diodes PDZ10BGW/SOD123 SOD2</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/771-PDZ10BGWX</t>
+  </si>
+  <si>
+    <t>SOT123</t>
+  </si>
+  <si>
+    <t>PDZ10BGWX</t>
+  </si>
+  <si>
+    <t>DCDC_1</t>
+  </si>
+  <si>
+    <t>EC4SBW-48S12</t>
+  </si>
+  <si>
+    <t>DCDC_20W_EC4SBW-48S12</t>
+  </si>
+  <si>
+    <t>Isolated DC/DC Converters DC-DC Converter, 20 Watt, 4:1 Input Range, 12VDC Output, 18-75VDC Input, 1670mA max., 1650uF</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/418-EC4SBW48S12</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>0.5A_FUSE</t>
+  </si>
+  <si>
+    <t>FUSE12-6</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>10K</t>
+  </si>
+  <si>
+    <t>RESISTOR_100K_0805-0805-1/8W-1%</t>
+  </si>
+  <si>
+    <t>Thick Film Resistors - SMD 0805 100Kohms 1% AEC-Q200</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/667-ERJ-6ENF1003V</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ERJ-6ENF1003V</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>PMOS_BSP322PH6327XTSA1</t>
+  </si>
+  <si>
+    <t>PMOS</t>
+  </si>
+  <si>
+    <t>MOSFET P-Ch -100V 1A SOT-223-3</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/726-BSP322PH6327XTSA</t>
+  </si>
+  <si>
+    <t>SOT-223</t>
+  </si>
+  <si>
+    <t>BSP322PH6327XTSA1</t>
+  </si>
+  <si>
+    <t>Surface Mount Fuses 1206 SMT Fuse VeryFastActing500mA</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Bel-Fuse/C1Q-500?qs=sGAEpiMZZMtxU2g%2F1juGqUe1nfAlZffAyIMgrBGBGxsQDVi%2Fw0PCPA%3D%3D</t>
+  </si>
+  <si>
+    <t>C1Q 500</t>
   </si>
 </sst>
 </file>
@@ -877,10 +956,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J38"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="K39" sqref="K39"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -921,7 +1000,7 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -941,7 +1020,7 @@
         <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G2" t="s">
         <v>18</v>
@@ -959,142 +1038,142 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>145</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>146</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>147</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>104</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>103</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G3" t="s">
-        <v>24</v>
+        <v>102</v>
       </c>
       <c r="H3">
-        <v>0.62</v>
+        <v>0.19</v>
       </c>
       <c r="I3">
         <v>2</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J37" si="0">H3*I3</f>
-        <v>1.24</v>
+        <f>H3*I3</f>
+        <v>0.38</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>148</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>146</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>147</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>104</v>
       </c>
       <c r="E4" t="s">
-        <v>29</v>
+        <v>103</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G4" t="s">
-        <v>30</v>
+        <v>102</v>
       </c>
       <c r="H4">
-        <v>0.08</v>
+        <v>0.19</v>
       </c>
       <c r="I4">
         <v>2</v>
       </c>
       <c r="J4">
-        <f t="shared" si="0"/>
-        <v>0.16</v>
+        <f>H4*I4</f>
+        <v>0.38</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G5" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="H5">
-        <v>7.2999999999999995E-2</v>
+        <v>0.62</v>
       </c>
       <c r="I5">
         <v>2</v>
       </c>
       <c r="J5">
-        <f t="shared" si="0"/>
-        <v>0.14599999999999999</v>
+        <f>H5*I5</f>
+        <v>1.24</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G6" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="H6">
-        <v>0.62</v>
+        <v>0.08</v>
       </c>
       <c r="I6">
         <v>2</v>
       </c>
       <c r="J6">
-        <f t="shared" si="0"/>
-        <v>1.24</v>
+        <f>H6*I6</f>
+        <v>0.16</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
         <v>15</v>
@@ -1106,7 +1185,7 @@
         <v>17</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G7" t="s">
         <v>18</v>
@@ -1118,178 +1197,178 @@
         <v>2</v>
       </c>
       <c r="J7">
-        <f t="shared" si="0"/>
+        <f>H7*I7</f>
         <v>0.14599999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E8" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G8" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="H8">
-        <v>0.08</v>
+        <v>0.62</v>
       </c>
       <c r="I8">
         <v>2</v>
       </c>
       <c r="J8">
-        <f t="shared" si="0"/>
-        <v>0.16</v>
+        <f>H8*I8</f>
+        <v>1.24</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="E9" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G9" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="H9">
-        <v>0.08</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="I9">
         <v>2</v>
       </c>
       <c r="J9">
-        <f t="shared" si="0"/>
-        <v>0.16</v>
+        <f>H9*I9</f>
+        <v>0.14599999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="E10" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G10" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="H10">
-        <v>7.2999999999999995E-2</v>
+        <v>0.08</v>
       </c>
       <c r="I10">
         <v>2</v>
       </c>
       <c r="J10">
-        <f t="shared" si="0"/>
-        <v>0.14599999999999999</v>
+        <f>H10*I10</f>
+        <v>0.16</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>150</v>
+        <v>37</v>
       </c>
       <c r="B11" t="s">
-        <v>151</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>152</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>109</v>
+        <v>28</v>
       </c>
       <c r="E11" t="s">
-        <v>108</v>
+        <v>29</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G11" t="s">
-        <v>107</v>
+        <v>30</v>
       </c>
       <c r="H11">
-        <v>0.19</v>
+        <v>0.08</v>
       </c>
       <c r="I11">
         <v>2</v>
       </c>
       <c r="J11">
-        <f t="shared" si="0"/>
-        <v>0.38</v>
+        <f>H11*I11</f>
+        <v>0.16</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>153</v>
+        <v>38</v>
       </c>
       <c r="B12" t="s">
-        <v>151</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>152</v>
+        <v>15</v>
       </c>
       <c r="D12" t="s">
-        <v>109</v>
+        <v>16</v>
       </c>
       <c r="E12" t="s">
-        <v>108</v>
+        <v>17</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G12" t="s">
-        <v>107</v>
+        <v>18</v>
       </c>
       <c r="H12">
-        <v>0.19</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="I12">
         <v>2</v>
       </c>
       <c r="J12">
-        <f t="shared" si="0"/>
-        <v>0.38</v>
+        <f>H12*I12</f>
+        <v>0.14599999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B13" t="s">
         <v>8</v>
@@ -1316,13 +1395,13 @@
         <v>1</v>
       </c>
       <c r="J13">
-        <f t="shared" si="0"/>
+        <f>H13*I13</f>
         <v>0.99</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B14" t="s">
         <v>8</v>
@@ -1349,13 +1428,13 @@
         <v>2</v>
       </c>
       <c r="J14">
-        <f t="shared" si="0"/>
+        <f>H14*I14</f>
         <v>1.98</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B15" t="s">
         <v>46</v>
@@ -1382,13 +1461,13 @@
         <v>2</v>
       </c>
       <c r="J15">
-        <f t="shared" si="0"/>
+        <f>H15*I15</f>
         <v>1.84</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B16" t="s">
         <v>51</v>
@@ -1415,13 +1494,13 @@
         <v>1</v>
       </c>
       <c r="J16">
-        <f t="shared" si="0"/>
+        <f>H16*I16</f>
         <v>0.84</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B17" t="s">
         <v>51</v>
@@ -1448,362 +1527,386 @@
         <v>2</v>
       </c>
       <c r="J17">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="J17:J41" si="0">H17*I17</f>
         <v>1.68</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" t="s">
+        <v>40</v>
+      </c>
       <c r="C18" t="s">
-        <v>134</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>138</v>
+        <v>109</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>139</v>
+        <v>41</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="H18">
-        <v>0.27</v>
+        <v>0.44</v>
       </c>
       <c r="I18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J18">
         <f t="shared" si="0"/>
-        <v>0.81</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>149</v>
+      </c>
+      <c r="B19" t="s">
+        <v>150</v>
+      </c>
       <c r="C19" t="s">
-        <v>135</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>140</v>
+        <v>151</v>
+      </c>
+      <c r="D19" t="s">
+        <v>152</v>
+      </c>
+      <c r="E19" t="s">
+        <v>153</v>
+      </c>
+      <c r="F19" t="s">
+        <v>154</v>
+      </c>
+      <c r="G19" t="s">
+        <v>155</v>
       </c>
       <c r="H19">
-        <v>0.23</v>
+        <v>0.16</v>
       </c>
       <c r="I19">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J19">
         <f t="shared" si="0"/>
-        <v>0.46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>156</v>
+      </c>
+      <c r="B20" t="s">
+        <v>157</v>
+      </c>
       <c r="C20" t="s">
-        <v>136</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>142</v>
+        <v>158</v>
+      </c>
+      <c r="D20" t="s">
+        <v>159</v>
+      </c>
+      <c r="E20" t="s">
+        <v>160</v>
+      </c>
+      <c r="F20"/>
+      <c r="G20" t="s">
+        <v>157</v>
       </c>
       <c r="H20">
-        <v>0.26</v>
+        <v>34</v>
       </c>
       <c r="I20">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J20">
         <f t="shared" si="0"/>
-        <v>0.78</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" t="s">
+        <v>45</v>
+      </c>
       <c r="C21" t="s">
-        <v>137</v>
-      </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="6" t="s">
-        <v>145</v>
+        <v>110</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>146</v>
+        <v>125</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="H21">
-        <v>5.1999999999999998E-2</v>
+        <v>0.8</v>
       </c>
       <c r="I21">
-        <v>100</v>
+        <v>2</v>
       </c>
       <c r="J21">
         <f t="shared" si="0"/>
-        <v>5.2</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>39</v>
+        <v>161</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>162</v>
       </c>
       <c r="C22" t="s">
-        <v>114</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>43</v>
+        <v>163</v>
+      </c>
+      <c r="D22" t="s">
+        <v>177</v>
+      </c>
+      <c r="E22" t="s">
+        <v>178</v>
+      </c>
+      <c r="F22">
+        <v>1206</v>
+      </c>
+      <c r="G22" t="s">
+        <v>179</v>
       </c>
       <c r="H22">
-        <v>0.44</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="I22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J22">
         <f t="shared" si="0"/>
-        <v>0.88</v>
+        <v>0.86999999999999988</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="C23" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>85</v>
+        <v>59</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>130</v>
+        <v>58</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="H23">
-        <v>0.8</v>
+        <v>4.5</v>
       </c>
       <c r="I23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J23">
         <f t="shared" si="0"/>
-        <v>1.6</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B24" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C24" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>57</v>
+        <v>85</v>
       </c>
       <c r="H24">
-        <v>4.5</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="I24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J24">
         <f t="shared" si="0"/>
-        <v>4.5</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B25" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C25" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>88</v>
+        <v>114</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>127</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="H25">
-        <v>1.1000000000000001</v>
+        <v>2.14</v>
       </c>
       <c r="I25">
         <v>2</v>
       </c>
       <c r="J25">
         <f t="shared" si="0"/>
-        <v>2.2000000000000002</v>
+        <v>4.28</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B26" t="s">
-        <v>63</v>
+        <v>89</v>
       </c>
       <c r="C26" t="s">
-        <v>118</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>64</v>
+        <v>115</v>
+      </c>
+      <c r="D26" t="s">
+        <v>88</v>
+      </c>
+      <c r="E26" t="s">
+        <v>87</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G26" t="s">
+        <v>89</v>
       </c>
       <c r="H26">
-        <v>2.14</v>
+        <v>0.49</v>
       </c>
       <c r="I26">
         <v>2</v>
       </c>
       <c r="J26">
         <f t="shared" si="0"/>
-        <v>4.28</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>65</v>
-      </c>
-      <c r="B27" t="s">
-        <v>94</v>
+        <v>67</v>
       </c>
       <c r="C27" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D27" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="E27" t="s">
-        <v>92</v>
+        <v>126</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G27" t="s">
-        <v>94</v>
+        <v>126</v>
       </c>
       <c r="H27">
-        <v>0.49</v>
+        <v>0</v>
       </c>
       <c r="I27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J27">
         <f t="shared" si="0"/>
-        <v>0.98</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>67</v>
+        <v>118</v>
+      </c>
+      <c r="B28" t="s">
+        <v>68</v>
       </c>
       <c r="C28" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D28" t="s">
-        <v>122</v>
+        <v>69</v>
       </c>
       <c r="E28" t="s">
-        <v>131</v>
+        <v>90</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>131</v>
+        <v>124</v>
+      </c>
+      <c r="G28" t="s">
+        <v>91</v>
       </c>
       <c r="H28">
-        <v>0</v>
+        <v>0.17599999999999999</v>
       </c>
       <c r="I28">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J28">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.52800000000000002</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B29" t="s">
         <v>68</v>
       </c>
       <c r="C29" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="D29" t="s">
         <v>69</v>
       </c>
       <c r="E29" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G29" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="H29">
         <v>0.17599999999999999</v>
@@ -1818,91 +1921,91 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>125</v>
-      </c>
-      <c r="B30" t="s">
-        <v>68</v>
+        <v>70</v>
+      </c>
+      <c r="B30">
+        <v>4.99</v>
       </c>
       <c r="C30" t="s">
+        <v>121</v>
+      </c>
+      <c r="D30" t="s">
+        <v>94</v>
+      </c>
+      <c r="E30" t="s">
+        <v>93</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="D30" t="s">
-        <v>69</v>
-      </c>
-      <c r="E30" t="s">
+      <c r="G30" t="s">
         <v>95</v>
       </c>
-      <c r="F30" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="G30" t="s">
-        <v>96</v>
-      </c>
       <c r="H30">
-        <v>0.17599999999999999</v>
+        <v>0.1</v>
       </c>
       <c r="I30">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J30">
         <f t="shared" si="0"/>
-        <v>0.52800000000000002</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>70</v>
-      </c>
-      <c r="B31">
-        <v>4.99</v>
+        <v>164</v>
+      </c>
+      <c r="B31" t="s">
+        <v>165</v>
       </c>
       <c r="C31" t="s">
-        <v>126</v>
+        <v>166</v>
       </c>
       <c r="D31" t="s">
-        <v>99</v>
+        <v>167</v>
       </c>
       <c r="E31" t="s">
-        <v>98</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>129</v>
+        <v>168</v>
+      </c>
+      <c r="F31">
+        <v>805</v>
       </c>
       <c r="G31" t="s">
-        <v>100</v>
+        <v>169</v>
       </c>
       <c r="H31">
         <v>0.1</v>
       </c>
       <c r="I31">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J31">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>0.30000000000000004</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B32" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C32" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D32" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E32" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="G32" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="H32">
         <v>0.44</v>
@@ -1923,19 +2026,19 @@
         <v>72</v>
       </c>
       <c r="C33" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D33" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E33" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>73</v>
       </c>
       <c r="G33" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="H33">
         <v>0.1</v>
@@ -1956,19 +2059,19 @@
         <v>72</v>
       </c>
       <c r="C34" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D34" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E34" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>73</v>
       </c>
       <c r="G34" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="H34">
         <v>0.1</v>
@@ -1989,19 +2092,19 @@
         <v>68</v>
       </c>
       <c r="C35" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="D35" t="s">
         <v>69</v>
       </c>
       <c r="E35" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G35" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="H35">
         <v>0.17599999999999999</v>
@@ -2016,82 +2119,207 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>76</v>
+        <v>170</v>
       </c>
       <c r="B36" t="s">
-        <v>68</v>
+        <v>171</v>
       </c>
       <c r="C36" t="s">
-        <v>124</v>
+        <v>172</v>
       </c>
       <c r="D36" t="s">
-        <v>69</v>
+        <v>173</v>
       </c>
       <c r="E36" t="s">
-        <v>95</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>129</v>
+        <v>174</v>
+      </c>
+      <c r="F36" t="s">
+        <v>175</v>
       </c>
       <c r="G36" t="s">
-        <v>96</v>
+        <v>176</v>
       </c>
       <c r="H36">
-        <v>0.17599999999999999</v>
+        <v>0.72</v>
       </c>
       <c r="I36">
         <v>2</v>
       </c>
       <c r="J36">
         <f t="shared" si="0"/>
-        <v>0.35199999999999998</v>
+        <v>1.44</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B37" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="C37" t="s">
-        <v>78</v>
+        <v>119</v>
       </c>
       <c r="D37" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="E37" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="G37" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="H37">
-        <v>25.44</v>
+        <v>0.17599999999999999</v>
       </c>
       <c r="I37">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J37">
         <f t="shared" si="0"/>
-        <v>25.44</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+        <v>0.35199999999999998</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="C38" t="s">
+        <v>129</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="H38">
+        <v>0.27</v>
+      </c>
+      <c r="I38">
+        <v>3</v>
+      </c>
       <c r="J38">
-        <f>SUM(J2:J37)</f>
-        <v>62.444000000000003</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="C39" t="s">
+        <v>130</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="H39">
+        <v>0.23</v>
+      </c>
+      <c r="I39">
+        <v>2</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="0"/>
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="C40" t="s">
+        <v>131</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="H40">
+        <v>0.26</v>
+      </c>
+      <c r="I40">
+        <v>3</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="0"/>
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="C41" t="s">
+        <v>132</v>
+      </c>
+      <c r="D41" s="2"/>
+      <c r="E41" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="H41">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="I41">
+        <v>100</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="0"/>
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J43">
+        <f>SUM(J2:J42)</f>
+        <v>74.094000000000008</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F45"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F46"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F47"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F48"/>
+    </row>
+    <row r="49" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F49"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:A49"/>
+  <sortState ref="A2:K41">
+    <sortCondition ref="A2"/>
+  </sortState>
   <hyperlinks>
-    <hyperlink ref="E18" r:id="rId1"/>
-    <hyperlink ref="E19" r:id="rId2"/>
-    <hyperlink ref="E20" r:id="rId3"/>
-    <hyperlink ref="E21" r:id="rId4"/>
+    <hyperlink ref="E38" r:id="rId1"/>
+    <hyperlink ref="E39" r:id="rId2"/>
+    <hyperlink ref="E40" r:id="rId3"/>
+    <hyperlink ref="E41" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>